<commit_message>
Updated testcases (Phase-2 New CR changes)
</commit_message>
<xml_diff>
--- a/testdata/ExcelTestData/Newtestdata.xlsx
+++ b/testdata/ExcelTestData/Newtestdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20356"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20337"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shakuntala\Periscope\pandc\testdata\ExcelTestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Shakuntala\Periscope\pandc\testdata\ExcelTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9074FCA5-B97A-4863-BFC5-2FB0FA43BB26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9371F5FE-3032-4667-89EA-126F4E00BDC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{D923499C-DDE5-4EE4-B604-8A52F010599A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="6" activeTab="9" xr2:uid="{D923499C-DDE5-4EE4-B604-8A52F010599A}"/>
   </bookViews>
   <sheets>
     <sheet name="CoverPage" sheetId="20" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <sheet name="Premium history " sheetId="1" r:id="rId21"/>
     <sheet name="Crime" sheetId="5" r:id="rId22"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="712">
   <si>
     <t>Column Name</t>
   </si>
@@ -1796,9 +1796,6 @@
     <t>Test Street</t>
   </si>
   <si>
-    <t>Test Company  2</t>
-  </si>
-  <si>
     <t>Test Street  2</t>
   </si>
   <si>
@@ -2232,6 +2229,12 @@
   </si>
   <si>
     <t>Test Info</t>
+  </si>
+  <si>
+    <t>Test Company 2</t>
+  </si>
+  <si>
+    <t>abcd@</t>
   </si>
 </sst>
 </file>
@@ -2467,7 +2470,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2637,12 +2640,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 4" xfId="1" builtinId="19"/>
@@ -2961,7 +2967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48ED3C3E-F680-454C-8DD3-367FA26F8D89}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2976,20 +2982,20 @@
         <v>25</v>
       </c>
       <c r="B1" s="54" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>305</v>
@@ -3000,23 +3006,23 @@
         <v>254</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
   </sheetData>
@@ -3026,10 +3032,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7386B1F8-159A-49CF-ACED-F12B36D938AD}">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3038,9 +3044,11 @@
     <col min="2" max="2" width="38.28515625" style="8" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" style="8" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="67"/>
+    <col min="10" max="12" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3048,12 +3056,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>148</v>
       </c>
@@ -3066,8 +3074,26 @@
       <c r="D3">
         <v>10000</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="85" t="s">
+        <v>711</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>711</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>711</v>
+      </c>
+      <c r="J3" s="84">
+        <v>12345678912365</v>
+      </c>
+      <c r="K3" s="84">
+        <v>12345678912365</v>
+      </c>
+      <c r="L3" s="84">
+        <v>12345678912365</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>149</v>
       </c>
@@ -3080,8 +3106,26 @@
       <c r="D4">
         <v>10000000</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="6" t="s">
+        <v>711</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>711</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>711</v>
+      </c>
+      <c r="J4" s="84">
+        <v>12345678912365</v>
+      </c>
+      <c r="K4" s="84">
+        <v>12345678912365</v>
+      </c>
+      <c r="L4" s="84">
+        <v>12345678912365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>150</v>
       </c>
@@ -3092,17 +3136,17 @@
         <v>18000000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>152</v>
       </c>
@@ -3110,7 +3154,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>153</v>
       </c>
@@ -3118,12 +3162,12 @@
         <v>19500</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>154</v>
       </c>
@@ -3131,7 +3175,7 @@
         <v>18500</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>155</v>
       </c>
@@ -3139,7 +3183,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>156</v>
       </c>
@@ -3147,7 +3191,7 @@
         <v>17500</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>157</v>
       </c>
@@ -3155,7 +3199,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>158</v>
       </c>
@@ -3163,7 +3207,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>159</v>
       </c>
@@ -3668,7 +3712,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{08716E94-C74C-454F-9918-6A6544CA63AD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3694,15 +3742,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B3">
         <v>120000</v>
@@ -3957,10 +4005,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B3" s="67" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C3" s="67"/>
       <c r="D3" s="67"/>
@@ -3970,7 +4018,7 @@
         <v>56</v>
       </c>
       <c r="B4" s="67" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C4" s="46"/>
       <c r="D4" s="67"/>
@@ -3980,7 +4028,7 @@
         <v>55</v>
       </c>
       <c r="B5" s="67" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C5" s="46"/>
       <c r="D5" s="67"/>
@@ -3990,7 +4038,7 @@
         <v>57</v>
       </c>
       <c r="B6" s="67" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C6" s="46"/>
       <c r="D6" s="67"/>
@@ -4016,10 +4064,10 @@
     </row>
     <row r="9" spans="1:6" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="72" t="s">
+        <v>593</v>
+      </c>
+      <c r="B9" s="67" t="s">
         <v>594</v>
-      </c>
-      <c r="B9" s="67" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -4035,7 +4083,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="72" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B11" s="22">
         <v>1</v>
@@ -4046,7 +4094,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B12" s="67">
         <v>8000</v>
@@ -4057,7 +4105,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="72" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B13" s="22">
         <v>1</v>
@@ -4068,7 +4116,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="72" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B14">
         <v>9000</v>
@@ -4079,7 +4127,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="72" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B15" s="22">
         <v>1</v>
@@ -4090,7 +4138,7 @@
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="72" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B16">
         <v>12</v>
@@ -4101,7 +4149,7 @@
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B17">
         <v>12000</v>
@@ -4112,7 +4160,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="72" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B18">
         <v>365</v>
@@ -4201,10 +4249,10 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="81"/>
+      <c r="B6" s="82"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
@@ -4368,10 +4416,10 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="81" t="s">
+      <c r="A26" s="82" t="s">
         <v>125</v>
       </c>
-      <c r="B26" s="81"/>
+      <c r="B26" s="82"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -4855,7 +4903,7 @@
         <v>251</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -5250,7 +5298,7 @@
         <v>443</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C2" s="41"/>
       <c r="D2" s="41"/>
@@ -5270,7 +5318,7 @@
         <v>57</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C4" s="41"/>
       <c r="D4" s="41"/>
@@ -5303,10 +5351,10 @@
     </row>
     <row r="7" spans="1:4" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="72" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B7" s="67" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="41" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -5314,7 +5362,7 @@
         <v>449</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -5663,7 +5711,7 @@
         <v>251</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C12" s="15"/>
     </row>
@@ -6336,7 +6384,7 @@
         <v>382</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C6" s="15"/>
     </row>
@@ -6398,7 +6446,7 @@
       <c r="C13" s="15"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="82" t="s">
+      <c r="A14" s="83" t="s">
         <v>393</v>
       </c>
       <c r="B14" s="30">
@@ -6407,7 +6455,7 @@
       <c r="C14" s="15"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="82"/>
+      <c r="A15" s="83"/>
       <c r="B15" s="30">
         <v>15</v>
       </c>
@@ -6971,10 +7019,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
+        <v>587</v>
+      </c>
+      <c r="B2" s="55" t="s">
         <v>588</v>
-      </c>
-      <c r="B2" s="55" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -6982,15 +7030,15 @@
         <v>56</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
+        <v>590</v>
+      </c>
+      <c r="B4" s="55" t="s">
         <v>591</v>
-      </c>
-      <c r="B4" s="55" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -7011,7 +7059,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B7" s="55" t="s">
         <v>69</v>
@@ -7019,15 +7067,15 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
+        <v>593</v>
+      </c>
+      <c r="B8" s="55" t="s">
         <v>594</v>
-      </c>
-      <c r="B8" s="55" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B9" s="78">
         <v>15000</v>
@@ -7035,7 +7083,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B10" s="78">
         <v>10000</v>
@@ -7043,7 +7091,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B11" s="78">
         <v>10000</v>
@@ -7067,7 +7115,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B14" s="78">
         <v>10000</v>
@@ -7075,7 +7123,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B15" s="78">
         <v>10000</v>
@@ -7083,7 +7131,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="59" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B16" s="78">
         <v>10000</v>
@@ -7091,7 +7139,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B17" s="78">
         <v>10000</v>
@@ -7099,7 +7147,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="58" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B18" s="78">
         <v>10000</v>
@@ -7107,7 +7155,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="58" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B19" s="78">
         <v>10000</v>
@@ -7115,7 +7163,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="58" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B20" s="78">
         <v>10000</v>
@@ -7123,7 +7171,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="58" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B21" s="78">
         <v>10000</v>
@@ -7131,7 +7179,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B22" s="78">
         <v>10000</v>
@@ -7139,7 +7187,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="58" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B23" s="78">
         <v>10000</v>
@@ -7147,7 +7195,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="58" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B24" s="78">
         <v>10000</v>
@@ -7155,7 +7203,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="58" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B25" s="78">
         <v>10000</v>
@@ -7163,7 +7211,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="58" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B26" s="78">
         <v>10000</v>
@@ -7171,7 +7219,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="58" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B27" s="78">
         <v>10000</v>
@@ -7179,7 +7227,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="58" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B28" s="78">
         <v>10000</v>
@@ -7187,7 +7235,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="58" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B29" s="78">
         <v>10000</v>
@@ -7195,7 +7243,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="58" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B30" s="78">
         <v>10000</v>
@@ -7203,7 +7251,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="58" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B31" s="78">
         <v>10000</v>
@@ -7211,7 +7259,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="58" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B32" s="78">
         <v>10000</v>
@@ -7219,7 +7267,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="58" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B33" s="78">
         <v>10000</v>
@@ -7227,7 +7275,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="58" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B34" s="78">
         <v>10000</v>
@@ -7235,7 +7283,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="58" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B35" s="78">
         <v>10000</v>
@@ -7243,7 +7291,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="58" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B36" s="78">
         <v>10000</v>
@@ -7251,7 +7299,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="58" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B37" s="78">
         <v>10000</v>
@@ -7291,7 +7339,7 @@
     </row>
     <row r="42" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="58" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B42" s="78">
         <v>45000</v>
@@ -7342,10 +7390,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="58" t="s">
+        <v>622</v>
+      </c>
+      <c r="B48" s="55" t="s">
         <v>623</v>
-      </c>
-      <c r="B48" s="55" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -7366,15 +7414,15 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="58" t="s">
+        <v>624</v>
+      </c>
+      <c r="B51" s="55" t="s">
         <v>625</v>
-      </c>
-      <c r="B51" s="55" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="58" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B52" s="55">
         <v>1000</v>
@@ -7390,7 +7438,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="58" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B54" s="55">
         <v>80</v>
@@ -7406,7 +7454,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="58" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B56" s="55">
         <v>15</v>
@@ -8046,7 +8094,7 @@
         <v>65</v>
       </c>
       <c r="B42" s="41" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -8100,8 +8148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D2AA5C-E1C4-4CA2-AB01-8B2F45BFCDB3}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8128,26 +8176,26 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="67" t="s">
+        <v>677</v>
+      </c>
+      <c r="B3" s="67" t="s">
         <v>678</v>
-      </c>
-      <c r="B3" s="67" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="67" t="s">
+        <v>679</v>
+      </c>
+      <c r="B4" s="67" t="s">
         <v>680</v>
-      </c>
-      <c r="B4" s="67" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="67" t="s">
+        <v>681</v>
+      </c>
+      <c r="B5" s="67" t="s">
         <v>682</v>
-      </c>
-      <c r="B5" s="67" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -8200,7 +8248,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="67" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B12" s="75">
         <v>10000</v>
@@ -8208,7 +8256,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="67" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B13" s="71">
         <v>0.2</v>
@@ -8219,23 +8267,23 @@
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="72" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B14" s="70">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="67" t="s">
-        <v>687</v>
-      </c>
-      <c r="B15" s="75">
+      <c r="A15" s="4" t="s">
+        <v>686</v>
+      </c>
+      <c r="B15" s="81">
         <v>10000</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="67" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B16" s="73">
         <v>3</v>
@@ -8243,10 +8291,10 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="67" t="s">
+        <v>688</v>
+      </c>
+      <c r="B17" s="67" t="s">
         <v>689</v>
-      </c>
-      <c r="B17" s="67" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -8254,7 +8302,7 @@
         <v>65</v>
       </c>
       <c r="B18" s="67" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -8335,10 +8383,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="82" t="s">
         <v>504</v>
       </c>
-      <c r="B2" s="81"/>
+      <c r="B2" s="82"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
@@ -8357,10 +8405,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="82" t="s">
         <v>507</v>
       </c>
-      <c r="B5" s="81"/>
+      <c r="B5" s="82"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
@@ -8387,10 +8435,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="81" t="s">
+      <c r="A9" s="82" t="s">
         <v>512</v>
       </c>
-      <c r="B9" s="81"/>
+      <c r="B9" s="82"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
@@ -9006,7 +9054,7 @@
         <v>548</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -9014,12 +9062,12 @@
         <v>549</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="55" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B4" s="55" t="s">
         <v>79</v>
@@ -9027,15 +9075,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
+        <v>574</v>
+      </c>
+      <c r="B5" s="55" t="s">
         <v>575</v>
-      </c>
-      <c r="B5" s="55" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="55" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B6" s="55" t="s">
         <v>79</v>
@@ -9046,23 +9094,23 @@
         <v>557</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="55" t="s">
+        <v>578</v>
+      </c>
+      <c r="B8" s="55" t="s">
         <v>579</v>
-      </c>
-      <c r="B8" s="55" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="55" t="s">
+        <v>580</v>
+      </c>
+      <c r="B9" s="55" t="s">
         <v>581</v>
-      </c>
-      <c r="B9" s="55" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -9075,7 +9123,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="55" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B11" s="55" t="s">
         <v>537</v>
@@ -9086,12 +9134,12 @@
         <v>560</v>
       </c>
       <c r="B12" s="55" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="55" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B13" s="55" t="s">
         <v>79</v>
@@ -9099,7 +9147,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="55" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B14" s="55" t="s">
         <v>79</v>
@@ -9110,7 +9158,7 @@
         <v>558</v>
       </c>
       <c r="B15" s="55" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
   </sheetData>
@@ -9123,7 +9171,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9218,7 +9266,7 @@
         <v>82</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>565</v>
+        <v>710</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -9226,7 +9274,7 @@
         <v>55</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -9234,7 +9282,7 @@
         <v>57</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -9250,7 +9298,7 @@
         <v>446</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -9298,7 +9346,7 @@
         <v>557</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -9306,7 +9354,7 @@
         <v>558</v>
       </c>
       <c r="B22" s="41" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -9322,7 +9370,7 @@
         <v>560</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
   </sheetData>
@@ -9358,7 +9406,7 @@
         <v>455</v>
       </c>
       <c r="B2" s="66" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -9366,7 +9414,7 @@
         <v>55</v>
       </c>
       <c r="B3" s="66" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -9374,7 +9422,7 @@
         <v>57</v>
       </c>
       <c r="B4" s="66" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -9395,15 +9443,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="63" t="s">
+        <v>593</v>
+      </c>
+      <c r="B7" s="66" t="s">
         <v>594</v>
-      </c>
-      <c r="B7" s="66" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="63" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B8" s="79">
         <v>10000</v>
@@ -9411,7 +9459,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="63" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B9" s="79">
         <v>10000</v>
@@ -9419,7 +9467,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B10" s="79">
         <v>10000</v>
@@ -9427,7 +9475,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="63" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B11" s="79">
         <v>10000</v>
@@ -9435,7 +9483,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="63" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B12" s="79">
         <v>10000</v>
@@ -9443,7 +9491,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B13" s="79">
         <v>10000</v>
@@ -9451,7 +9499,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="63" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B14" s="79">
         <v>10000</v>
@@ -9459,7 +9507,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B15" s="79">
         <v>10000</v>
@@ -9467,7 +9515,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="63" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B16" s="79">
         <v>10000</v>
@@ -9475,7 +9523,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="63" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B17" s="79">
         <v>10000</v>
@@ -9483,7 +9531,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="63" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B18" s="79">
         <v>10000</v>
@@ -9491,7 +9539,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="63" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B19" s="79">
         <v>10000</v>
@@ -9499,7 +9547,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="63" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B20" s="79">
         <v>10000</v>
@@ -9507,7 +9555,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="63" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B21" s="79">
         <v>10000</v>
@@ -9515,7 +9563,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="63" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B22" s="79">
         <v>10000</v>
@@ -9523,7 +9571,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="63" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B23" s="79">
         <v>10000</v>
@@ -9531,7 +9579,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="63" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B24" s="79">
         <v>10000</v>
@@ -9539,7 +9587,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="63" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B25" s="79">
         <v>10000</v>
@@ -9547,7 +9595,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="63" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B26" s="79">
         <v>10000</v>
@@ -9555,7 +9603,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="63" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B27" s="79">
         <v>10000</v>
@@ -9563,7 +9611,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="63" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B28" s="79">
         <v>10000</v>
@@ -9571,7 +9619,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="63" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B29" s="79">
         <v>10000</v>
@@ -9579,7 +9627,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="63" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B30" s="79">
         <v>10000</v>
@@ -9587,7 +9635,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="63" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B31" s="79">
         <v>10000</v>
@@ -9595,7 +9643,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="63" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B32" s="79">
         <v>10000</v>
@@ -9606,7 +9654,7 @@
         <v>62</v>
       </c>
       <c r="B33" s="66" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -9646,7 +9694,7 @@
         <v>65</v>
       </c>
       <c r="B38" s="66" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -9670,7 +9718,7 @@
         <v>557</v>
       </c>
       <c r="B41" s="66" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -9686,12 +9734,12 @@
         <v>486</v>
       </c>
       <c r="B43" s="66" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="63" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B44" s="66" t="s">
         <v>70</v>
@@ -9699,7 +9747,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="63" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B45" s="66" t="s">
         <v>79</v>
@@ -9707,7 +9755,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="63" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B46" s="66" t="s">
         <v>79</v>
@@ -9715,7 +9763,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="63" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B47" s="66" t="s">
         <v>79</v>
@@ -9723,15 +9771,15 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="63" t="s">
+        <v>654</v>
+      </c>
+      <c r="B48" s="66" t="s">
         <v>655</v>
-      </c>
-      <c r="B48" s="66" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="63" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B49" s="66" t="s">
         <v>79</v>
@@ -9739,7 +9787,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="63" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B50" s="66" t="s">
         <v>79</v>
@@ -9747,15 +9795,15 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="63" t="s">
+        <v>658</v>
+      </c>
+      <c r="B51" s="66" t="s">
         <v>659</v>
-      </c>
-      <c r="B51" s="66" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="63" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B52" s="66" t="s">
         <v>79</v>
@@ -9763,15 +9811,15 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="63" t="s">
+        <v>661</v>
+      </c>
+      <c r="B53" s="66" t="s">
         <v>662</v>
-      </c>
-      <c r="B53" s="66" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="63" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B54" s="66" t="s">
         <v>79</v>
@@ -9779,7 +9827,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="63" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B55" s="66" t="s">
         <v>79</v>
@@ -9787,39 +9835,39 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="63" t="s">
+        <v>665</v>
+      </c>
+      <c r="B56" s="66" t="s">
         <v>666</v>
-      </c>
-      <c r="B56" s="66" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="63" t="s">
+        <v>667</v>
+      </c>
+      <c r="B57" s="66" t="s">
         <v>668</v>
-      </c>
-      <c r="B57" s="66" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="63" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B58" s="66" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="63" t="s">
+        <v>670</v>
+      </c>
+      <c r="B59" s="66" t="s">
         <v>671</v>
-      </c>
-      <c r="B59" s="66" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="63" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B60" s="66" t="s">
         <v>79</v>
@@ -9827,7 +9875,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="63" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B61" s="66" t="s">
         <v>79</v>
@@ -9835,10 +9883,10 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="63" t="s">
+        <v>674</v>
+      </c>
+      <c r="B62" s="66" t="s">
         <v>675</v>
-      </c>
-      <c r="B62" s="66" t="s">
-        <v>676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated methods in excelOperation class
</commit_message>
<xml_diff>
--- a/testdata/ExcelTestData/Newtestdata.xlsx
+++ b/testdata/ExcelTestData/Newtestdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Shakuntala\Periscope\pandc\testdata\ExcelTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF91FA3-E950-454E-A4BC-3C63F0D83C68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60FBDB7-2A1D-4C12-AC06-A3BCB6CE5D8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="900" firstSheet="19" activeTab="25" xr2:uid="{D923499C-DDE5-4EE4-B604-8A52F010599A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="900" firstSheet="5" activeTab="8" xr2:uid="{D923499C-DDE5-4EE4-B604-8A52F010599A}"/>
   </bookViews>
   <sheets>
     <sheet name="CoverPage" sheetId="20" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1910" uniqueCount="786">
   <si>
     <t>Column Name</t>
   </si>
@@ -2458,6 +2458,15 @@
   <si>
     <t>Us Workers</t>
   </si>
+  <si>
+    <t>Product Revenues</t>
+  </si>
+  <si>
+    <t>Sales/Service Revenues</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
 </sst>
 </file>
 
@@ -2467,7 +2476,7 @@
     <numFmt numFmtId="164" formatCode="mm\/dd\/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd\/mm\/yyyy"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2606,6 +2615,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF172B4D"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -2764,7 +2779,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="185">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -3117,6 +3132,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3128,12 +3151,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3521,8 +3538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7386B1F8-159A-49CF-ACED-F12B36D938AD}">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5282,10 +5299,10 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="180" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="176"/>
+      <c r="B6" s="180"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -5449,10 +5466,10 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="176" t="s">
+      <c r="A26" s="180" t="s">
         <v>125</v>
       </c>
-      <c r="B26" s="176"/>
+      <c r="B26" s="180"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -5782,8 +5799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80E40C2-8F61-422B-8B66-5E35CD325EB0}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6324,8 +6341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6855AF93-82AA-4D05-A803-46C5BBC6D83F}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6677,7 +6694,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6866,8 +6883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84AE8549-2611-4C3D-8F42-2BE39C7FE28A}">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7682,7 +7699,7 @@
       <c r="D13" s="165"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="179" t="s">
+      <c r="A14" s="183" t="s">
         <v>389</v>
       </c>
       <c r="B14" s="29">
@@ -7694,7 +7711,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="179"/>
+      <c r="A15" s="183"/>
       <c r="B15" s="29">
         <v>15</v>
       </c>
@@ -8411,16 +8428,16 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{079DEC00-3AA1-408E-BD73-5592DDC980E2}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -8457,61 +8474,149 @@
     </row>
     <row r="5" spans="1:4" s="169" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="182" t="s">
+      <c r="A6" s="184" t="s">
         <v>782</v>
       </c>
-      <c r="B6" s="182"/>
+      <c r="B6" s="184"/>
     </row>
     <row r="7" spans="1:4" ht="99" x14ac:dyDescent="0.25">
-      <c r="A7" s="180" t="s">
+      <c r="A7" s="176" t="s">
         <v>778</v>
       </c>
-      <c r="B7" s="181">
+      <c r="B7" s="177">
         <v>10</v>
       </c>
-      <c r="C7" s="180"/>
-      <c r="D7" s="180"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
     </row>
     <row r="8" spans="1:4" ht="82.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="180" t="s">
+      <c r="A8" s="176" t="s">
         <v>779</v>
       </c>
-      <c r="B8" s="181">
+      <c r="B8" s="177">
         <v>10</v>
       </c>
-      <c r="C8" s="180"/>
-      <c r="D8" s="180"/>
+      <c r="C8" s="176"/>
+      <c r="D8" s="176"/>
     </row>
     <row r="9" spans="1:4" ht="99" x14ac:dyDescent="0.25">
-      <c r="A9" s="180" t="s">
+      <c r="A9" s="176" t="s">
         <v>780</v>
       </c>
-      <c r="B9" s="181">
+      <c r="B9" s="177">
         <v>10</v>
       </c>
-      <c r="C9" s="181">
+      <c r="C9" s="177">
         <v>1000</v>
       </c>
-      <c r="D9" s="180"/>
+      <c r="D9" s="176"/>
     </row>
     <row r="10" spans="1:4" ht="82.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="180" t="s">
+      <c r="A10" s="176" t="s">
         <v>781</v>
       </c>
-      <c r="B10" s="181">
+      <c r="B10" s="177">
         <v>10</v>
       </c>
-      <c r="C10" s="181">
+      <c r="C10" s="177">
         <v>1000</v>
       </c>
-      <c r="D10" s="180"/>
+      <c r="D10" s="176"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="146" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="162" t="s">
+        <v>479</v>
+      </c>
+      <c r="B12" s="178">
+        <v>12.233000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="162" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="179">
+        <v>123456789123654</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="162" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="179">
+        <v>123456789123654</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="162" t="s">
+        <v>595</v>
+      </c>
+      <c r="B15" s="179">
+        <v>123456789123654</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="162" t="s">
+        <v>596</v>
+      </c>
+      <c r="B16" s="179">
+        <v>123456789123654</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="162" t="s">
+        <v>597</v>
+      </c>
+      <c r="B17" s="179">
+        <v>123456789123654</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="162" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="179">
+        <v>123456789123654</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="176" t="s">
+        <v>783</v>
+      </c>
+      <c r="B19" s="179">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="176" t="s">
+        <v>784</v>
+      </c>
+      <c r="B20" s="179">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="176" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="176" t="s">
+        <v>785</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8519,8 +8624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327F0A58-02FC-4F22-8797-343AD32130AA}">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10474,14 +10579,14 @@
       <c r="L1" s="131"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="180" t="s">
         <v>500</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="J2" s="177" t="s">
+      <c r="B2" s="180"/>
+      <c r="J2" s="181" t="s">
         <v>500</v>
       </c>
-      <c r="K2" s="177"/>
+      <c r="K2" s="181"/>
       <c r="L2" s="131"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -10511,14 +10616,14 @@
       <c r="L4" s="131"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="180" t="s">
         <v>503</v>
       </c>
-      <c r="B5" s="176"/>
-      <c r="J5" s="177" t="s">
+      <c r="B5" s="180"/>
+      <c r="J5" s="181" t="s">
         <v>503</v>
       </c>
-      <c r="K5" s="177"/>
+      <c r="K5" s="181"/>
       <c r="L5" s="131"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -10555,14 +10660,14 @@
       <c r="L8" s="131"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="180" t="s">
         <v>508</v>
       </c>
-      <c r="B9" s="176"/>
-      <c r="J9" s="178" t="s">
+      <c r="B9" s="180"/>
+      <c r="J9" s="182" t="s">
         <v>508</v>
       </c>
-      <c r="K9" s="178"/>
+      <c r="K9" s="182"/>
       <c r="L9" s="131"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -11809,8 +11914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93FDE03-E8E3-44A0-BF55-9C72F1DA2A4D}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11931,7 +12036,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="166" t="s">
         <v>598</v>
       </c>
       <c r="B11" s="84">
@@ -11967,7 +12072,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="166" t="s">
         <v>601</v>
       </c>
       <c r="B14" s="84">
@@ -12015,7 +12120,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="81" t="s">
+      <c r="A18" s="166" t="s">
         <v>605</v>
       </c>
       <c r="B18" s="84">
@@ -12073,7 +12178,7 @@
       <c r="D22" s="143"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="81" t="s">
+      <c r="A23" s="166" t="s">
         <v>609</v>
       </c>
       <c r="B23" s="84">

</xml_diff>

<commit_message>
- Added new scripts into WebTest.java - Added data into Newtestdata.xlsx - Updated build version into app.properties
</commit_message>
<xml_diff>
--- a/testdata/ExcelTestData/Newtestdata.xlsx
+++ b/testdata/ExcelTestData/Newtestdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Shakuntala\Periscope\pandc\testdata\ExcelTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6F3B3F-DBBA-4D5B-B7FD-9AC28D25647C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCF1C12-A307-429F-9122-F65262A84E01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="900" firstSheet="19" activeTab="25" xr2:uid="{D923499C-DDE5-4EE4-B604-8A52F010599A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="900" firstSheet="1" activeTab="2" xr2:uid="{D923499C-DDE5-4EE4-B604-8A52F010599A}"/>
   </bookViews>
   <sheets>
     <sheet name="CoverPage" sheetId="20" r:id="rId1"/>
@@ -44,7 +44,7 @@
     <definedName name="country_list">#REF!</definedName>
     <definedName name="us_states">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1552" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="793">
   <si>
     <t>Column Name</t>
   </si>
@@ -2484,6 +2484,9 @@
   </si>
   <si>
     <t># of Days Coverage for Ordinary Payroll Desired (0 - 365 days)</t>
+  </si>
+  <si>
+    <t>Revenue By Location</t>
   </si>
 </sst>
 </file>
@@ -6583,7 +6586,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAE12E4D-FB7F-4E63-97F0-B0D0FFCBC628}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8448,7 +8453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{079DEC00-3AA1-408E-BD73-5592DDC980E2}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -8772,10 +8777,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327F0A58-02FC-4F22-8797-343AD32130AA}">
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9787,6 +9792,17 @@
       <c r="C93" s="64"/>
       <c r="D93" s="109" t="s">
         <v>715</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A94" s="175" t="s">
+        <v>792</v>
+      </c>
+      <c r="B94" s="175">
+        <v>10000</v>
+      </c>
+      <c r="D94" t="s">
+        <v>746</v>
       </c>
     </row>
   </sheetData>
@@ -10406,8 +10422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D2AA5C-E1C4-4CA2-AB01-8B2F45BFCDB3}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>